<commit_message>
New Qgis project for locations
</commit_message>
<xml_diff>
--- a/notes/Calculation_Livestock.xlsx
+++ b/notes/Calculation_Livestock.xlsx
@@ -8,12 +8,13 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jonat\Documents\Master EE\03_Steppingstone\05_Project\Volta-burkina-faso\notes\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{2102B7BC-E377-4346-86A1-17C65E48B27E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E4DFF523-E46F-4E08-A7AF-4288F5A554F7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="10718" yWindow="0" windowWidth="10965" windowHeight="12863" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="10718" yWindow="0" windowWidth="10965" windowHeight="12863" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="page-1_table-1" sheetId="1" r:id="rId1"/>
+    <sheet name="Irrigation" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -33,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="133" uniqueCount="98">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="147" uniqueCount="98">
   <si>
     <t>Region</t>
   </si>
@@ -716,8 +717,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:T14"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="L1" workbookViewId="0">
-      <selection activeCell="T5" sqref="T5:T14"/>
+    <sheetView topLeftCell="Q1" workbookViewId="0">
+      <selection activeCell="S1" sqref="S1:S14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.5"/>
@@ -1531,4 +1532,187 @@
     <ignoredError sqref="B1:H14" numberStoredAsText="1"/>
   </ignoredErrors>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C3D96AB6-F0D5-4BFA-95B3-AF675CA8E837}">
+  <dimension ref="B4:D17"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F8" sqref="F8"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.5"/>
+  <cols>
+    <col min="2" max="2" width="17.75" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="4" spans="2:4" x14ac:dyDescent="0.5">
+      <c r="B4" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="C4" s="1">
+        <v>2001</v>
+      </c>
+      <c r="D4" s="1">
+        <v>2023</v>
+      </c>
+    </row>
+    <row r="5" spans="2:4" x14ac:dyDescent="0.5">
+      <c r="B5" t="s">
+        <v>7</v>
+      </c>
+      <c r="C5">
+        <v>4391</v>
+      </c>
+      <c r="D5">
+        <f>C5*2</f>
+        <v>8782</v>
+      </c>
+    </row>
+    <row r="6" spans="2:4" x14ac:dyDescent="0.5">
+      <c r="B6" t="s">
+        <v>14</v>
+      </c>
+      <c r="D6">
+        <f t="shared" ref="D6:D17" si="0">C6*2</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="7" spans="2:4" x14ac:dyDescent="0.5">
+      <c r="B7" t="s">
+        <v>21</v>
+      </c>
+      <c r="C7">
+        <v>1495</v>
+      </c>
+      <c r="D7">
+        <f t="shared" si="0"/>
+        <v>2990</v>
+      </c>
+    </row>
+    <row r="8" spans="2:4" x14ac:dyDescent="0.5">
+      <c r="B8" t="s">
+        <v>28</v>
+      </c>
+      <c r="C8">
+        <v>2210</v>
+      </c>
+      <c r="D8">
+        <f t="shared" si="0"/>
+        <v>4420</v>
+      </c>
+    </row>
+    <row r="9" spans="2:4" x14ac:dyDescent="0.5">
+      <c r="B9" t="s">
+        <v>35</v>
+      </c>
+      <c r="C9">
+        <v>1135</v>
+      </c>
+      <c r="D9">
+        <f t="shared" si="0"/>
+        <v>2270</v>
+      </c>
+    </row>
+    <row r="10" spans="2:4" x14ac:dyDescent="0.5">
+      <c r="B10" t="s">
+        <v>42</v>
+      </c>
+      <c r="C10">
+        <v>555</v>
+      </c>
+      <c r="D10">
+        <f t="shared" si="0"/>
+        <v>1110</v>
+      </c>
+    </row>
+    <row r="11" spans="2:4" x14ac:dyDescent="0.5">
+      <c r="B11" t="s">
+        <v>49</v>
+      </c>
+      <c r="C11">
+        <v>2210</v>
+      </c>
+      <c r="D11">
+        <f t="shared" si="0"/>
+        <v>4420</v>
+      </c>
+    </row>
+    <row r="12" spans="2:4" x14ac:dyDescent="0.5">
+      <c r="B12" t="s">
+        <v>56</v>
+      </c>
+      <c r="C12">
+        <v>580</v>
+      </c>
+      <c r="D12">
+        <f t="shared" si="0"/>
+        <v>1160</v>
+      </c>
+    </row>
+    <row r="13" spans="2:4" x14ac:dyDescent="0.5">
+      <c r="B13" t="s">
+        <v>63</v>
+      </c>
+      <c r="C13">
+        <v>13165</v>
+      </c>
+      <c r="D13">
+        <f t="shared" si="0"/>
+        <v>26330</v>
+      </c>
+    </row>
+    <row r="14" spans="2:4" x14ac:dyDescent="0.5">
+      <c r="B14" t="s">
+        <v>70</v>
+      </c>
+      <c r="C14">
+        <v>875</v>
+      </c>
+      <c r="D14">
+        <f t="shared" si="0"/>
+        <v>1750</v>
+      </c>
+    </row>
+    <row r="15" spans="2:4" x14ac:dyDescent="0.5">
+      <c r="B15" t="s">
+        <v>77</v>
+      </c>
+      <c r="C15">
+        <v>1700</v>
+      </c>
+      <c r="D15">
+        <f t="shared" si="0"/>
+        <v>3400</v>
+      </c>
+    </row>
+    <row r="16" spans="2:4" x14ac:dyDescent="0.5">
+      <c r="B16" t="s">
+        <v>83</v>
+      </c>
+      <c r="C16">
+        <v>270</v>
+      </c>
+      <c r="D16">
+        <f t="shared" si="0"/>
+        <v>540</v>
+      </c>
+    </row>
+    <row r="17" spans="2:4" x14ac:dyDescent="0.5">
+      <c r="B17" t="s">
+        <v>90</v>
+      </c>
+      <c r="C17">
+        <v>325</v>
+      </c>
+      <c r="D17">
+        <f t="shared" si="0"/>
+        <v>650</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>